<commit_message>
new resources from dzop
</commit_message>
<xml_diff>
--- a/lm-be-communication.xlsx
+++ b/lm-be-communication.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AI$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AI$19</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="118">
   <si>
     <t>Path</t>
   </si>
@@ -144,6 +144,58 @@
     <t>The Communication object represents a message sent or note entered in a diary, in the context of care.</t>
   </si>
   <si>
+    <t>BECommunication.id</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
+</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>BECommunication.extension</t>
+  </si>
+  <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
     <t>BECommunication.identifier</t>
   </si>
   <si>
@@ -163,9 +215,6 @@
     <t>BECommunication.status</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t xml:space="preserve">code {code}
 </t>
   </si>
@@ -285,7 +334,7 @@
     <t>BECommunication.context.patient</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(BEPatient)
+    <t xml:space="preserve">Reference(https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/be-patient)
 </t>
   </si>
   <si>
@@ -485,7 +534,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AI17"/>
+  <dimension ref="A1:AI19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -496,7 +545,7 @@
   <cols>
     <col min="1" max="1" width="36.0078125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
@@ -521,10 +570,10 @@
     <col min="25" max="25" width="46.078125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="10.0546875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="31" max="31" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
@@ -731,7 +780,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
         <v>42</v>
       </c>
@@ -744,10 +793,10 @@
         <v>37</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s" s="2">
         <v>36</v>
@@ -812,11 +861,15 @@
       <c r="AD3" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="AE3" s="2"/>
+      <c r="AE3" t="s" s="2">
+        <v>47</v>
+      </c>
       <c r="AF3" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="AG3" s="2"/>
+      <c r="AG3" t="s" s="2">
+        <v>43</v>
+      </c>
       <c r="AH3" t="s" s="2">
         <v>36</v>
       </c>
@@ -824,23 +877,23 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s" s="2">
         <v>36</v>
@@ -849,15 +902,17 @@
         <v>36</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="M4" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="M4" t="s" s="2">
+        <v>53</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
         <v>36</v>
@@ -894,22 +949,26 @@
         <v>36</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="AC4" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AE4" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="AE4" t="s" s="2">
+        <v>57</v>
+      </c>
       <c r="AF4" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="AG4" s="2"/>
+      <c r="AG4" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="AH4" t="s" s="2">
         <v>36</v>
       </c>
@@ -919,7 +978,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -930,10 +989,10 @@
         <v>37</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>36</v>
@@ -942,13 +1001,13 @@
         <v>36</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1012,7 +1071,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1020,13 +1079,13 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s" s="2">
         <v>36</v>
@@ -1035,13 +1094,13 @@
         <v>36</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1103,9 +1162,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" hidden="true">
+    <row r="7">
       <c r="A7" t="s" s="2">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
@@ -1116,10 +1175,10 @@
         <v>37</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s" s="2">
         <v>36</v>
@@ -1128,13 +1187,13 @@
         <v>36</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1196,9 +1255,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" hidden="true">
+    <row r="8">
       <c r="A8" t="s" s="2">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -1212,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H8" t="s" s="2">
         <v>36</v>
@@ -1221,13 +1280,13 @@
         <v>36</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1289,9 +1348,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -1305,7 +1364,7 @@
         <v>38</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H9" t="s" s="2">
         <v>36</v>
@@ -1314,13 +1373,13 @@
         <v>36</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1384,7 +1443,7 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -1407,13 +1466,13 @@
         <v>36</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1475,9 +1534,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" hidden="true">
+    <row r="11">
       <c r="A11" t="s" s="2">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -1491,7 +1550,7 @@
         <v>38</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>36</v>
@@ -1500,13 +1559,13 @@
         <v>36</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1533,13 +1592,13 @@
         <v>36</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="Z11" t="s" s="2">
         <v>36</v>
@@ -1570,7 +1629,7 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -1593,13 +1652,13 @@
         <v>36</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1663,7 +1722,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -1686,13 +1745,13 @@
         <v>36</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1719,13 +1778,13 @@
         <v>36</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>36</v>
@@ -1754,9 +1813,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -1770,7 +1829,7 @@
         <v>38</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>36</v>
@@ -1779,13 +1838,13 @@
         <v>36</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1849,7 +1908,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -1872,13 +1931,13 @@
         <v>36</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1940,9 +1999,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -1956,7 +2015,7 @@
         <v>38</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>36</v>
@@ -1968,10 +2027,10 @@
         <v>97</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2035,7 +2094,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2058,13 +2117,13 @@
         <v>36</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2126,8 +2185,194 @@
         <v>36</v>
       </c>
     </row>
+    <row r="18" hidden="true">
+      <c r="A18" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="I18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="J18" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="K18" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="L18" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="P18" s="2"/>
+      <c r="Q18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="R18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="S18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="T18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="U18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="V18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="W18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="X18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Y18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Z18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AB18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AC18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AD18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AE18" s="2"/>
+      <c r="AF18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG18" s="2"/>
+      <c r="AH18" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AI18" t="s" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" hidden="true">
+      <c r="A19" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="I19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="J19" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K19" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="L19" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="R19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="S19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="T19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="U19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="V19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="W19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="X19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Y19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Z19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AB19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AC19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AD19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AE19" s="2"/>
+      <c r="AF19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG19" s="2"/>
+      <c r="AH19" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AI19" t="s" s="2">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AI17">
+  <autoFilter ref="A1:AI19">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -2137,7 +2382,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI16">
+  <conditionalFormatting sqref="A2:AI18">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Work on string320, fix qa issues
</commit_message>
<xml_diff>
--- a/lm-be-communication.xlsx
+++ b/lm-be-communication.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AI$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AI$20</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="121">
   <si>
     <t>Path</t>
   </si>
@@ -260,6 +260,15 @@
     <t>What is the trigger data element for this communication - whether it is an updated medication, or an encounter...</t>
   </si>
   <si>
+    <t>BECommunication.partOf</t>
+  </si>
+  <si>
+    <t>The broader communication that this communication is a part of</t>
+  </si>
+  <si>
+    <t>This will be used in multi-part messages, namely for when the content is beyond the character limit</t>
+  </si>
+  <si>
     <t>BECommunication.inReponseTo</t>
   </si>
   <si>
@@ -356,7 +365,7 @@
     <t>BECommunication.content.text</t>
   </si>
   <si>
-    <t xml:space="preserve">Annotation {https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/structuredefinition-be-annotation320}
+    <t xml:space="preserve">Annotation {https://www.ehealth.fgov.be/standards/fhir/StructureDefinition/string320}
 </t>
   </si>
   <si>
@@ -534,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AI19"/>
+  <dimension ref="A1:AI20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1466,13 +1475,13 @@
         <v>36</v>
       </c>
       <c r="J10" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K10" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="K10" t="s" s="2">
+      <c r="L10" t="s" s="2">
         <v>80</v>
-      </c>
-      <c r="L10" t="s" s="2">
-        <v>81</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1534,9 +1543,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -1550,7 +1559,7 @@
         <v>38</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>36</v>
@@ -1559,10 +1568,10 @@
         <v>36</v>
       </c>
       <c r="J11" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="K11" t="s" s="2">
         <v>83</v>
-      </c>
-      <c r="K11" t="s" s="2">
-        <v>84</v>
       </c>
       <c r="L11" t="s" s="2">
         <v>84</v>
@@ -1627,7 +1636,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" hidden="true">
+    <row r="12">
       <c r="A12" t="s" s="2">
         <v>85</v>
       </c>
@@ -1643,7 +1652,7 @@
         <v>38</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>36</v>
@@ -1658,7 +1667,7 @@
         <v>87</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1722,7 +1731,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -1745,13 +1754,13 @@
         <v>36</v>
       </c>
       <c r="J13" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="K13" t="s" s="2">
         <v>90</v>
       </c>
-      <c r="K13" t="s" s="2">
+      <c r="L13" t="s" s="2">
         <v>91</v>
-      </c>
-      <c r="L13" t="s" s="2">
-        <v>92</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1778,13 +1787,13 @@
         <v>36</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>36</v>
@@ -1815,7 +1824,7 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -1838,13 +1847,13 @@
         <v>36</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1871,13 +1880,13 @@
         <v>36</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>36</v>
@@ -1908,7 +1917,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -1931,13 +1940,13 @@
         <v>36</v>
       </c>
       <c r="J15" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="K15" t="s" s="2">
         <v>101</v>
       </c>
-      <c r="K15" t="s" s="2">
+      <c r="L15" t="s" s="2">
         <v>102</v>
-      </c>
-      <c r="L15" t="s" s="2">
-        <v>103</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1999,9 +2008,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2015,7 +2024,7 @@
         <v>38</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>36</v>
@@ -2024,7 +2033,7 @@
         <v>36</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="K16" t="s" s="2">
         <v>105</v>
@@ -2092,7 +2101,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
         <v>107</v>
       </c>
@@ -2108,7 +2117,7 @@
         <v>38</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>36</v>
@@ -2117,13 +2126,13 @@
         <v>36</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="L17" t="s" s="2">
-        <v>110</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2187,7 +2196,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2210,13 +2219,13 @@
         <v>36</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>113</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>114</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2280,7 +2289,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -2303,7 +2312,7 @@
         <v>36</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="K19" t="s" s="2">
         <v>116</v>
@@ -2371,8 +2380,101 @@
         <v>36</v>
       </c>
     </row>
+    <row r="20" hidden="true">
+      <c r="A20" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="I20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="J20" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="L20" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="P20" s="2"/>
+      <c r="Q20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="R20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="S20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="T20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="U20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="V20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="W20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="X20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Y20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Z20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AB20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AC20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AD20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AE20" s="2"/>
+      <c r="AF20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG20" s="2"/>
+      <c r="AH20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AI20" t="s" s="2">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AI19">
+  <autoFilter ref="A1:AI20">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -2382,7 +2484,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI18">
+  <conditionalFormatting sqref="A2:AI19">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>